<commit_message>
Frotinha ajustado, fazendo o ajuste
</commit_message>
<xml_diff>
--- a/data/qff_cpi_3.xlsx
+++ b/data/qff_cpi_3.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\frotinha\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2166,16 +2172,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
-      <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2194,49 +2201,373 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:49">
       <c r="G1" s="5" t="s">
         <v>643</v>
       </c>
@@ -2246,11 +2577,11 @@
       <c r="I1" s="5" t="s">
         <v>647</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
       <c r="M1" s="5" t="s">
         <v>653</v>
       </c>
@@ -2260,30 +2591,30 @@
       <c r="O1" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
       <c r="U1" s="5" t="s">
         <v>666</v>
       </c>
       <c r="V1" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5" t="s">
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
       <c r="AB1" s="5" t="s">
         <v>677</v>
       </c>
@@ -2293,19 +2624,19 @@
       <c r="AD1" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
       <c r="AP1" s="5" t="s">
         <v>695</v>
       </c>
@@ -2327,11 +2658,11 @@
       <c r="AV1" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="7" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:49" ht="138.75">
       <c r="A2" s="6" t="s">
         <v>710</v>
       </c>
@@ -2476,11 +2807,11 @@
       <c r="AV2" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="AW2" s="5" t="s">
+      <c r="AW2" s="7" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:49">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2547,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:49">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2624,7 +2955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:49">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2695,7 +3026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:49">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2762,11 +3093,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:49">
+      <c r="A7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2829,10 +3160,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="1:49">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2904,10 +3235,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
+    <row r="9" spans="1:49">
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2981,10 +3312,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
+    <row r="10" spans="1:49">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
@@ -3046,10 +3377,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:49">
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
@@ -3121,11 +3452,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:49">
+      <c r="A12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -3192,10 +3523,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="1" t="s">
+    <row r="13" spans="1:49">
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -3273,10 +3604,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:49">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="1" t="s">
         <v>50</v>
       </c>
@@ -3352,7 +3683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:49">
       <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
@@ -3423,7 +3754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:49">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -3502,7 +3833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:49">
       <c r="A17" s="2" t="s">
         <v>71</v>
       </c>
@@ -3585,7 +3916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:49">
       <c r="A18" s="2" t="s">
         <v>77</v>
       </c>
@@ -3652,7 +3983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:49">
       <c r="A19" s="2" t="s">
         <v>83</v>
       </c>
@@ -3719,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:49">
       <c r="A20" s="2" t="s">
         <v>89</v>
       </c>
@@ -3790,7 +4121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:49">
       <c r="A21" s="2" t="s">
         <v>95</v>
       </c>
@@ -3857,7 +4188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:49">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -3924,7 +4255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:49">
       <c r="A23" s="2" t="s">
         <v>107</v>
       </c>
@@ -3995,7 +4326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:49">
       <c r="A24" s="2" t="s">
         <v>113</v>
       </c>
@@ -4062,7 +4393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:49">
       <c r="A25" s="2" t="s">
         <v>119</v>
       </c>
@@ -4129,7 +4460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:49">
       <c r="A26" s="2" t="s">
         <v>125</v>
       </c>
@@ -4198,7 +4529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:49">
       <c r="A27" s="2" t="s">
         <v>131</v>
       </c>
@@ -4265,7 +4596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:49">
       <c r="A28" s="2" t="s">
         <v>137</v>
       </c>
@@ -4336,7 +4667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:49">
       <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
@@ -4403,7 +4734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:49">
       <c r="A30" s="2" t="s">
         <v>149</v>
       </c>
@@ -4474,7 +4805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:49">
       <c r="A31" s="2" t="s">
         <v>155</v>
       </c>
@@ -4541,7 +4872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:49">
       <c r="A32" s="2" t="s">
         <v>161</v>
       </c>
@@ -4608,7 +4939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:49">
       <c r="A33" s="2" t="s">
         <v>167</v>
       </c>
@@ -4675,7 +5006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:49">
       <c r="A34" s="2" t="s">
         <v>173</v>
       </c>
@@ -4742,7 +5073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:49">
       <c r="A35" s="2" t="s">
         <v>179</v>
       </c>
@@ -4809,11 +5140,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:49">
+      <c r="A36" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="9" t="s">
         <v>196</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -4876,10 +5207,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="1" t="s">
+    <row r="37" spans="1:49">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="8" t="s">
         <v>195</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -4953,10 +5284,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="1"/>
+    <row r="38" spans="1:49">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="1" t="s">
         <v>189</v>
       </c>
@@ -5028,10 +5359,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="1"/>
+    <row r="39" spans="1:49">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="1" t="s">
         <v>192</v>
       </c>
@@ -5091,10 +5422,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="1"/>
+    <row r="40" spans="1:49">
+      <c r="A40" s="10"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="1" t="s">
         <v>194</v>
       </c>
@@ -5168,7 +5499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:49">
       <c r="A41" s="2" t="s">
         <v>203</v>
       </c>
@@ -5235,7 +5566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:49">
       <c r="A42" s="2" t="s">
         <v>209</v>
       </c>
@@ -5314,7 +5645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:49">
       <c r="A43" s="2" t="s">
         <v>215</v>
       </c>
@@ -5385,7 +5716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:49">
       <c r="A44" s="2" t="s">
         <v>221</v>
       </c>
@@ -5452,7 +5783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:49">
       <c r="A45" s="2" t="s">
         <v>227</v>
       </c>
@@ -5523,7 +5854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:49">
       <c r="A46" s="2" t="s">
         <v>233</v>
       </c>
@@ -5590,7 +5921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:49">
       <c r="A47" s="2" t="s">
         <v>239</v>
       </c>
@@ -5661,7 +5992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:49">
       <c r="A48" s="2" t="s">
         <v>245</v>
       </c>
@@ -5746,7 +6077,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:49">
       <c r="A49" s="2" t="s">
         <v>251</v>
       </c>
@@ -5817,7 +6148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:49">
       <c r="A50" s="2" t="s">
         <v>257</v>
       </c>
@@ -5884,7 +6215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:49">
       <c r="A51" s="2" t="s">
         <v>263</v>
       </c>
@@ -5957,7 +6288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:49">
       <c r="A52" s="2" t="s">
         <v>269</v>
       </c>
@@ -6024,7 +6355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:49">
       <c r="A53" s="2" t="s">
         <v>275</v>
       </c>
@@ -6103,7 +6434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:49">
       <c r="A54" s="2" t="s">
         <v>281</v>
       </c>
@@ -6170,7 +6501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:49">
       <c r="A55" s="2" t="s">
         <v>287</v>
       </c>
@@ -6253,7 +6584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:49">
       <c r="A56" s="2" t="s">
         <v>293</v>
       </c>
@@ -6324,7 +6655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:49">
       <c r="A57" s="2" t="s">
         <v>299</v>
       </c>
@@ -6391,7 +6722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:49">
       <c r="A58" s="2" t="s">
         <v>305</v>
       </c>
@@ -6458,7 +6789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:49">
       <c r="A59" s="2" t="s">
         <v>311</v>
       </c>
@@ -6541,7 +6872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:49">
       <c r="A60" s="2" t="s">
         <v>317</v>
       </c>
@@ -6612,7 +6943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:49">
       <c r="A61" s="2" t="s">
         <v>323</v>
       </c>
@@ -6685,7 +7016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:49">
       <c r="A62" s="2" t="s">
         <v>329</v>
       </c>
@@ -6752,7 +7083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:49">
       <c r="A63" s="2" t="s">
         <v>335</v>
       </c>
@@ -6823,7 +7154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:49">
       <c r="A64" s="2" t="s">
         <v>341</v>
       </c>
@@ -6890,7 +7221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:49">
       <c r="A65" s="2" t="s">
         <v>347</v>
       </c>
@@ -6957,7 +7288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:49">
       <c r="A66" s="2" t="s">
         <v>353</v>
       </c>
@@ -7024,7 +7355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:49">
       <c r="A67" s="2" t="s">
         <v>359</v>
       </c>
@@ -7105,7 +7436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:49">
       <c r="A68" s="2" t="s">
         <v>365</v>
       </c>
@@ -7182,7 +7513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:49">
       <c r="A69" s="2" t="s">
         <v>371</v>
       </c>
@@ -7249,7 +7580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:49">
       <c r="A70" s="2" t="s">
         <v>377</v>
       </c>
@@ -7318,7 +7649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:49">
       <c r="A71" s="2" t="s">
         <v>383</v>
       </c>
@@ -7385,7 +7716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:49">
       <c r="A72" s="2" t="s">
         <v>389</v>
       </c>
@@ -7458,7 +7789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:49">
       <c r="A73" s="2" t="s">
         <v>395</v>
       </c>
@@ -7531,7 +7862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:49">
       <c r="A74" s="2" t="s">
         <v>401</v>
       </c>
@@ -7612,7 +7943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:49">
       <c r="A75" s="2" t="s">
         <v>407</v>
       </c>
@@ -7681,7 +8012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:49">
       <c r="A76" s="2" t="s">
         <v>413</v>
       </c>
@@ -7748,7 +8079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:49">
       <c r="A77" s="2" t="s">
         <v>419</v>
       </c>
@@ -7815,7 +8146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:49">
       <c r="A78" s="2" t="s">
         <v>425</v>
       </c>
@@ -7882,14 +8213,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="s">
+    <row r="79" spans="1:49">
+      <c r="A79" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="8" t="s">
         <v>437</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -7965,10 +8296,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="1"/>
+    <row r="80" spans="1:49">
+      <c r="A80" s="10"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="1" t="s">
         <v>431</v>
       </c>
@@ -8040,10 +8371,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="1"/>
+    <row r="81" spans="1:49">
+      <c r="A81" s="10"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="1" t="s">
         <v>434</v>
       </c>
@@ -8105,10 +8436,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="1"/>
+    <row r="82" spans="1:49">
+      <c r="A82" s="10"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="1" t="s">
         <v>436</v>
       </c>
@@ -8178,10 +8509,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="1" t="s">
+    <row r="83" spans="1:49">
+      <c r="A83" s="10"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="8" t="s">
         <v>446</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -8245,10 +8576,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="1"/>
+    <row r="84" spans="1:49">
+      <c r="A84" s="10"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="1" t="s">
         <v>443</v>
       </c>
@@ -8306,10 +8637,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="1"/>
+    <row r="85" spans="1:49">
+      <c r="A85" s="10"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="1" t="s">
         <v>445</v>
       </c>
@@ -8373,10 +8704,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="1" t="s">
+    <row r="86" spans="1:49">
+      <c r="A86" s="10"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="8" t="s">
         <v>461</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -8450,10 +8781,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="1"/>
+    <row r="87" spans="1:49">
+      <c r="A87" s="10"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="8"/>
       <c r="D87" s="1" t="s">
         <v>452</v>
       </c>
@@ -8527,10 +8858,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="1"/>
+    <row r="88" spans="1:49">
+      <c r="A88" s="10"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="1" t="s">
         <v>455</v>
       </c>
@@ -8606,10 +8937,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="1"/>
+    <row r="89" spans="1:49">
+      <c r="A89" s="10"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="1" t="s">
         <v>458</v>
       </c>
@@ -8671,10 +9002,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="1"/>
+    <row r="90" spans="1:49">
+      <c r="A90" s="10"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="8"/>
       <c r="D90" s="1" t="s">
         <v>460</v>
       </c>
@@ -8744,9 +9075,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2"/>
-      <c r="B91" s="3"/>
+    <row r="91" spans="1:49">
+      <c r="A91" s="10"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="1" t="s">
         <v>464</v>
       </c>
@@ -8831,7 +9162,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:49">
       <c r="A92" s="2" t="s">
         <v>471</v>
       </c>
@@ -8898,7 +9229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:49">
       <c r="A93" s="2" t="s">
         <v>477</v>
       </c>
@@ -8967,7 +9298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:49">
       <c r="A94" s="2" t="s">
         <v>483</v>
       </c>
@@ -9034,7 +9365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:49">
       <c r="A95" s="2" t="s">
         <v>489</v>
       </c>
@@ -9101,7 +9432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:49">
       <c r="A96" s="2" t="s">
         <v>495</v>
       </c>
@@ -9168,7 +9499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:49">
       <c r="A97" s="2" t="s">
         <v>501</v>
       </c>
@@ -9235,7 +9566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:49">
       <c r="A98" s="2" t="s">
         <v>507</v>
       </c>
@@ -9306,7 +9637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:49">
       <c r="A99" s="2" t="s">
         <v>513</v>
       </c>
@@ -9377,7 +9708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:49">
       <c r="A100" s="2" t="s">
         <v>519</v>
       </c>
@@ -9444,11 +9775,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:49">
+      <c r="A101" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="9" t="s">
         <v>536</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -9511,10 +9842,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="1" t="s">
+    <row r="102" spans="1:49">
+      <c r="A102" s="10"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="8" t="s">
         <v>535</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -9588,10 +9919,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="1"/>
+    <row r="103" spans="1:49">
+      <c r="A103" s="10"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="8"/>
       <c r="D103" s="1" t="s">
         <v>529</v>
       </c>
@@ -9663,10 +9994,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="1"/>
+    <row r="104" spans="1:49">
+      <c r="A104" s="10"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="8"/>
       <c r="D104" s="1" t="s">
         <v>532</v>
       </c>
@@ -9728,10 +10059,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="1"/>
+    <row r="105" spans="1:49">
+      <c r="A105" s="10"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="8"/>
       <c r="D105" s="1" t="s">
         <v>534</v>
       </c>
@@ -9803,7 +10134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:49">
       <c r="A106" s="2" t="s">
         <v>543</v>
       </c>
@@ -9876,7 +10207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:49">
       <c r="A107" s="2" t="s">
         <v>549</v>
       </c>
@@ -9943,7 +10274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:49">
       <c r="A108" s="2" t="s">
         <v>555</v>
       </c>
@@ -10022,7 +10353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:49">
       <c r="A109" s="2" t="s">
         <v>561</v>
       </c>
@@ -10093,7 +10424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:49">
       <c r="A110" s="2" t="s">
         <v>567</v>
       </c>
@@ -10164,11 +10495,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:49">
+      <c r="A111" s="10" t="s">
         <v>579</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="9" t="s">
         <v>578</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -10231,10 +10562,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="1" t="s">
+    <row r="112" spans="1:49">
+      <c r="A112" s="10"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="8" t="s">
         <v>577</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -10312,10 +10643,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="1"/>
+    <row r="113" spans="1:49">
+      <c r="A113" s="10"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="8"/>
       <c r="D113" s="1" t="s">
         <v>576</v>
       </c>
@@ -10385,7 +10716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:49">
       <c r="A114" s="2" t="s">
         <v>585</v>
       </c>
@@ -10452,7 +10783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:49">
       <c r="A115" s="2" t="s">
         <v>591</v>
       </c>
@@ -10521,7 +10852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:49">
       <c r="A116" s="2" t="s">
         <v>597</v>
       </c>
@@ -10588,7 +10919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:49">
       <c r="A117" s="2" t="s">
         <v>603</v>
       </c>
@@ -10655,7 +10986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:49">
       <c r="A118" s="2" t="s">
         <v>609</v>
       </c>
@@ -10722,7 +11053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:49">
       <c r="A119" s="2" t="s">
         <v>615</v>
       </c>
@@ -10805,7 +11136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:49">
       <c r="A120" s="2" t="s">
         <v>621</v>
       </c>
@@ -10872,7 +11203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:49">
       <c r="A121" s="2" t="s">
         <v>627</v>
       </c>
@@ -10939,7 +11270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:49">
       <c r="A122" s="2" t="s">
         <v>633</v>
       </c>
@@ -11006,7 +11337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:49">
       <c r="A123" s="2" t="s">
         <v>639</v>
       </c>
@@ -11073,23 +11404,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" s="2" t="s">
+    <row r="124" spans="1:49">
+      <c r="A124" s="10" t="s">
         <v>641</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F124" s="10" t="s">
         <v>640</v>
       </c>
       <c r="G124" s="3">
@@ -11210,28 +11541,29 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="A124:F124"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="C86:C90"/>
     <mergeCell ref="B79:B91"/>
     <mergeCell ref="A79:A91"/>
     <mergeCell ref="C102:C105"/>
     <mergeCell ref="B101:B105"/>
     <mergeCell ref="A101:A105"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="A124:F124"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="AW1:AW2"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="AE1:AO1"/>
-    <mergeCell ref="AW1:AW2"/>
   </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>